<commit_message>
lot of files changed
</commit_message>
<xml_diff>
--- a/Disease Excel Worksheet.xlsx
+++ b/Disease Excel Worksheet.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\HTN PROJECT 2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -321,34 +329,38 @@
     <t>Prostate Cancer</t>
   </si>
   <si>
-    <t>frequent urges to urinate;difficulty commencing anding maintain urination;blood in the urine;painful urination and ejaculation;difficulty achieving or maintaining an erection</t>
-  </si>
-  <si>
     <t>You may have prostate cancer, please consult with a doctor and conduct further diagnostics at your local hospital</t>
+  </si>
+  <si>
+    <t>frequent urges to urinate;difficulty commencing and maintaining urination;blood in the urine;painful urination and ejaculation;difficulty achieving or maintaining an erection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -358,7 +370,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -374,66 +386,337 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K995"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.71"/>
-    <col customWidth="1" min="2" max="2" width="27.43"/>
-    <col customWidth="1" min="3" max="3" width="29.43"/>
-    <col customWidth="1" min="4" max="4" width="27.86"/>
-    <col customWidth="1" min="5" max="5" width="32.43"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,9 +737,9 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -471,13 +754,13 @@
         <v>9</v>
       </c>
       <c r="F2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -492,12 +775,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A29" si="1">A3+1</f>
+        <f t="shared" ref="A4:A29" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -513,12 +796,12 @@
         <v>17</v>
       </c>
       <c r="F4" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -534,13 +817,13 @@
         <v>21</v>
       </c>
       <c r="F5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -556,13 +839,13 @@
         <v>25</v>
       </c>
       <c r="F6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -578,12 +861,12 @@
         <v>29</v>
       </c>
       <c r="F7" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -599,12 +882,12 @@
         <v>33</v>
       </c>
       <c r="F8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -620,12 +903,12 @@
         <v>37</v>
       </c>
       <c r="F9" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -639,13 +922,13 @@
         <v>40</v>
       </c>
       <c r="F10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -661,13 +944,13 @@
         <v>44</v>
       </c>
       <c r="F11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -683,13 +966,13 @@
         <v>48</v>
       </c>
       <c r="F12" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -705,13 +988,13 @@
         <v>52</v>
       </c>
       <c r="F13" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -725,13 +1008,13 @@
         <v>55</v>
       </c>
       <c r="F14" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -747,13 +1030,13 @@
         <v>59</v>
       </c>
       <c r="F15" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -769,13 +1052,13 @@
         <v>63</v>
       </c>
       <c r="F16" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -789,13 +1072,13 @@
         <v>66</v>
       </c>
       <c r="F17" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -809,13 +1092,13 @@
         <v>69</v>
       </c>
       <c r="F18" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -829,13 +1112,13 @@
         <v>72</v>
       </c>
       <c r="F19" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -851,13 +1134,13 @@
         <v>76</v>
       </c>
       <c r="F20" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -870,13 +1153,13 @@
         <v>79</v>
       </c>
       <c r="F21" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -890,13 +1173,13 @@
         <v>82</v>
       </c>
       <c r="F22" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -910,13 +1193,13 @@
         <v>85</v>
       </c>
       <c r="F23" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -930,13 +1213,13 @@
         <v>88</v>
       </c>
       <c r="F24" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -950,13 +1233,13 @@
         <v>91</v>
       </c>
       <c r="F25" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -970,13 +1253,13 @@
         <v>94</v>
       </c>
       <c r="F26" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -990,13 +1273,13 @@
         <v>97</v>
       </c>
       <c r="F27" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1010,2928 +1293,2928 @@
         <v>100</v>
       </c>
       <c r="F28" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F29" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K35" s="2"/>
     </row>
-    <row r="36">
+    <row r="36" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K36" s="2"/>
     </row>
-    <row r="37">
+    <row r="37" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K38" s="2"/>
     </row>
-    <row r="39">
+    <row r="39" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K39" s="2"/>
     </row>
-    <row r="40">
+    <row r="40" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K43" s="2"/>
     </row>
-    <row r="44">
+    <row r="44" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K45" s="2"/>
     </row>
-    <row r="46">
+    <row r="46" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K46" s="2"/>
     </row>
-    <row r="47">
+    <row r="47" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K47" s="2"/>
     </row>
-    <row r="48">
+    <row r="48" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K48" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K49" s="2"/>
     </row>
-    <row r="50">
+    <row r="50" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K50" s="2"/>
     </row>
-    <row r="51">
+    <row r="51" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K51" s="2"/>
     </row>
-    <row r="52">
+    <row r="52" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K52" s="2"/>
     </row>
-    <row r="53">
+    <row r="53" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K53" s="2"/>
     </row>
-    <row r="54">
+    <row r="54" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K54" s="2"/>
     </row>
-    <row r="55">
+    <row r="55" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K55" s="2"/>
     </row>
-    <row r="56">
+    <row r="56" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K58" s="2"/>
     </row>
-    <row r="59">
+    <row r="59" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K59" s="2"/>
     </row>
-    <row r="60">
+    <row r="60" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K60" s="2"/>
     </row>
-    <row r="61">
+    <row r="61" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K61" s="2"/>
     </row>
-    <row r="62">
+    <row r="62" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K62" s="2"/>
     </row>
-    <row r="63">
+    <row r="63" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K63" s="2"/>
     </row>
-    <row r="64">
+    <row r="64" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K65" s="2"/>
     </row>
-    <row r="66">
+    <row r="66" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K67" s="2"/>
     </row>
-    <row r="68">
+    <row r="68" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K68" s="2"/>
     </row>
-    <row r="69">
+    <row r="69" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K69" s="2"/>
     </row>
-    <row r="70">
+    <row r="70" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K70" s="2"/>
     </row>
-    <row r="71">
+    <row r="71" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K71" s="2"/>
     </row>
-    <row r="72">
+    <row r="72" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K72" s="2"/>
     </row>
-    <row r="73">
+    <row r="73" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K73" s="2"/>
     </row>
-    <row r="74">
+    <row r="74" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K74" s="2"/>
     </row>
-    <row r="75">
+    <row r="75" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K75" s="2"/>
     </row>
-    <row r="76">
+    <row r="76" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K76" s="2"/>
     </row>
-    <row r="77">
+    <row r="77" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K77" s="2"/>
     </row>
-    <row r="78">
+    <row r="78" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K78" s="2"/>
     </row>
-    <row r="79">
+    <row r="79" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K79" s="2"/>
     </row>
-    <row r="80">
+    <row r="80" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K80" s="2"/>
     </row>
-    <row r="81">
+    <row r="81" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K81" s="2"/>
     </row>
-    <row r="82">
+    <row r="82" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K82" s="2"/>
     </row>
-    <row r="83">
+    <row r="83" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K83" s="2"/>
     </row>
-    <row r="84">
+    <row r="84" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K84" s="2"/>
     </row>
-    <row r="85">
+    <row r="85" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K85" s="2"/>
     </row>
-    <row r="86">
+    <row r="86" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K86" s="2"/>
     </row>
-    <row r="87">
+    <row r="87" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K87" s="2"/>
     </row>
-    <row r="88">
+    <row r="88" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K88" s="2"/>
     </row>
-    <row r="89">
+    <row r="89" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K89" s="2"/>
     </row>
-    <row r="90">
+    <row r="90" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K90" s="2"/>
     </row>
-    <row r="91">
+    <row r="91" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K91" s="2"/>
     </row>
-    <row r="92">
+    <row r="92" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K92" s="2"/>
     </row>
-    <row r="93">
+    <row r="93" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K93" s="2"/>
     </row>
-    <row r="94">
+    <row r="94" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K94" s="2"/>
     </row>
-    <row r="95">
+    <row r="95" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K95" s="2"/>
     </row>
-    <row r="96">
+    <row r="96" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K96" s="2"/>
     </row>
-    <row r="97">
+    <row r="97" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K97" s="2"/>
     </row>
-    <row r="98">
+    <row r="98" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K98" s="2"/>
     </row>
-    <row r="99">
+    <row r="99" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K99" s="2"/>
     </row>
-    <row r="100">
+    <row r="100" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K100" s="2"/>
     </row>
-    <row r="101">
+    <row r="101" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K101" s="2"/>
     </row>
-    <row r="102">
+    <row r="102" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K102" s="2"/>
     </row>
-    <row r="103">
+    <row r="103" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K103" s="2"/>
     </row>
-    <row r="104">
+    <row r="104" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K104" s="2"/>
     </row>
-    <row r="105">
+    <row r="105" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K105" s="2"/>
     </row>
-    <row r="106">
+    <row r="106" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K106" s="2"/>
     </row>
-    <row r="107">
+    <row r="107" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K107" s="2"/>
     </row>
-    <row r="108">
+    <row r="108" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K108" s="2"/>
     </row>
-    <row r="109">
+    <row r="109" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K109" s="2"/>
     </row>
-    <row r="110">
+    <row r="110" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K110" s="2"/>
     </row>
-    <row r="111">
+    <row r="111" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K111" s="2"/>
     </row>
-    <row r="112">
+    <row r="112" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K112" s="2"/>
     </row>
-    <row r="113">
+    <row r="113" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K113" s="2"/>
     </row>
-    <row r="114">
+    <row r="114" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K114" s="2"/>
     </row>
-    <row r="115">
+    <row r="115" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K115" s="2"/>
     </row>
-    <row r="116">
+    <row r="116" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K116" s="2"/>
     </row>
-    <row r="117">
+    <row r="117" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K117" s="2"/>
     </row>
-    <row r="118">
+    <row r="118" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K118" s="2"/>
     </row>
-    <row r="119">
+    <row r="119" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K119" s="2"/>
     </row>
-    <row r="120">
+    <row r="120" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K120" s="2"/>
     </row>
-    <row r="121">
+    <row r="121" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K121" s="2"/>
     </row>
-    <row r="122">
+    <row r="122" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K122" s="2"/>
     </row>
-    <row r="123">
+    <row r="123" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K123" s="2"/>
     </row>
-    <row r="124">
+    <row r="124" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K124" s="2"/>
     </row>
-    <row r="125">
+    <row r="125" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K125" s="2"/>
     </row>
-    <row r="126">
+    <row r="126" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K126" s="2"/>
     </row>
-    <row r="127">
+    <row r="127" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K127" s="2"/>
     </row>
-    <row r="128">
+    <row r="128" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K128" s="2"/>
     </row>
-    <row r="129">
+    <row r="129" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K129" s="2"/>
     </row>
-    <row r="130">
+    <row r="130" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K130" s="2"/>
     </row>
-    <row r="131">
+    <row r="131" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K131" s="2"/>
     </row>
-    <row r="132">
+    <row r="132" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K132" s="2"/>
     </row>
-    <row r="133">
+    <row r="133" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K133" s="2"/>
     </row>
-    <row r="134">
+    <row r="134" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K134" s="2"/>
     </row>
-    <row r="135">
+    <row r="135" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K135" s="2"/>
     </row>
-    <row r="136">
+    <row r="136" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K136" s="2"/>
     </row>
-    <row r="137">
+    <row r="137" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K137" s="2"/>
     </row>
-    <row r="138">
+    <row r="138" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K138" s="2"/>
     </row>
-    <row r="139">
+    <row r="139" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K139" s="2"/>
     </row>
-    <row r="140">
+    <row r="140" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K140" s="2"/>
     </row>
-    <row r="141">
+    <row r="141" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K141" s="2"/>
     </row>
-    <row r="142">
+    <row r="142" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K142" s="2"/>
     </row>
-    <row r="143">
+    <row r="143" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K143" s="2"/>
     </row>
-    <row r="144">
+    <row r="144" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K144" s="2"/>
     </row>
-    <row r="145">
+    <row r="145" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K145" s="2"/>
     </row>
-    <row r="146">
+    <row r="146" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K146" s="2"/>
     </row>
-    <row r="147">
+    <row r="147" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K147" s="2"/>
     </row>
-    <row r="148">
+    <row r="148" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K148" s="2"/>
     </row>
-    <row r="149">
+    <row r="149" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K149" s="2"/>
     </row>
-    <row r="150">
+    <row r="150" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K150" s="2"/>
     </row>
-    <row r="151">
+    <row r="151" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K151" s="2"/>
     </row>
-    <row r="152">
+    <row r="152" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K152" s="2"/>
     </row>
-    <row r="153">
+    <row r="153" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K153" s="2"/>
     </row>
-    <row r="154">
+    <row r="154" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K154" s="2"/>
     </row>
-    <row r="155">
+    <row r="155" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K155" s="2"/>
     </row>
-    <row r="156">
+    <row r="156" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K156" s="2"/>
     </row>
-    <row r="157">
+    <row r="157" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K157" s="2"/>
     </row>
-    <row r="158">
+    <row r="158" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K158" s="2"/>
     </row>
-    <row r="159">
+    <row r="159" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K159" s="2"/>
     </row>
-    <row r="160">
+    <row r="160" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K160" s="2"/>
     </row>
-    <row r="161">
+    <row r="161" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K161" s="2"/>
     </row>
-    <row r="162">
+    <row r="162" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K162" s="2"/>
     </row>
-    <row r="163">
+    <row r="163" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K163" s="2"/>
     </row>
-    <row r="164">
+    <row r="164" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K164" s="2"/>
     </row>
-    <row r="165">
+    <row r="165" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K165" s="2"/>
     </row>
-    <row r="166">
+    <row r="166" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K166" s="2"/>
     </row>
-    <row r="167">
+    <row r="167" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K167" s="2"/>
     </row>
-    <row r="168">
+    <row r="168" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K168" s="2"/>
     </row>
-    <row r="169">
+    <row r="169" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K169" s="2"/>
     </row>
-    <row r="170">
+    <row r="170" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K170" s="2"/>
     </row>
-    <row r="171">
+    <row r="171" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K171" s="2"/>
     </row>
-    <row r="172">
+    <row r="172" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K172" s="2"/>
     </row>
-    <row r="173">
+    <row r="173" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K173" s="2"/>
     </row>
-    <row r="174">
+    <row r="174" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K174" s="2"/>
     </row>
-    <row r="175">
+    <row r="175" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K175" s="2"/>
     </row>
-    <row r="176">
+    <row r="176" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K176" s="2"/>
     </row>
-    <row r="177">
+    <row r="177" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K177" s="2"/>
     </row>
-    <row r="178">
+    <row r="178" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K178" s="2"/>
     </row>
-    <row r="179">
+    <row r="179" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K179" s="2"/>
     </row>
-    <row r="180">
+    <row r="180" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K180" s="2"/>
     </row>
-    <row r="181">
+    <row r="181" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K181" s="2"/>
     </row>
-    <row r="182">
+    <row r="182" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K182" s="2"/>
     </row>
-    <row r="183">
+    <row r="183" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K183" s="2"/>
     </row>
-    <row r="184">
+    <row r="184" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K184" s="2"/>
     </row>
-    <row r="185">
+    <row r="185" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K185" s="2"/>
     </row>
-    <row r="186">
+    <row r="186" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K186" s="2"/>
     </row>
-    <row r="187">
+    <row r="187" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K187" s="2"/>
     </row>
-    <row r="188">
+    <row r="188" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K188" s="2"/>
     </row>
-    <row r="189">
+    <row r="189" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K189" s="2"/>
     </row>
-    <row r="190">
+    <row r="190" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K190" s="2"/>
     </row>
-    <row r="191">
+    <row r="191" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K191" s="2"/>
     </row>
-    <row r="192">
+    <row r="192" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K192" s="2"/>
     </row>
-    <row r="193">
+    <row r="193" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K193" s="2"/>
     </row>
-    <row r="194">
+    <row r="194" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K194" s="2"/>
     </row>
-    <row r="195">
+    <row r="195" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K195" s="2"/>
     </row>
-    <row r="196">
+    <row r="196" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K196" s="2"/>
     </row>
-    <row r="197">
+    <row r="197" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K197" s="2"/>
     </row>
-    <row r="198">
+    <row r="198" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K198" s="2"/>
     </row>
-    <row r="199">
+    <row r="199" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K199" s="2"/>
     </row>
-    <row r="200">
+    <row r="200" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K200" s="2"/>
     </row>
-    <row r="201">
+    <row r="201" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K201" s="2"/>
     </row>
-    <row r="202">
+    <row r="202" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K202" s="2"/>
     </row>
-    <row r="203">
+    <row r="203" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K203" s="2"/>
     </row>
-    <row r="204">
+    <row r="204" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K204" s="2"/>
     </row>
-    <row r="205">
+    <row r="205" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K205" s="2"/>
     </row>
-    <row r="206">
+    <row r="206" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K206" s="2"/>
     </row>
-    <row r="207">
+    <row r="207" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K207" s="2"/>
     </row>
-    <row r="208">
+    <row r="208" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K208" s="2"/>
     </row>
-    <row r="209">
+    <row r="209" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K209" s="2"/>
     </row>
-    <row r="210">
+    <row r="210" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K210" s="2"/>
     </row>
-    <row r="211">
+    <row r="211" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K211" s="2"/>
     </row>
-    <row r="212">
+    <row r="212" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K212" s="2"/>
     </row>
-    <row r="213">
+    <row r="213" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K213" s="2"/>
     </row>
-    <row r="214">
+    <row r="214" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K214" s="2"/>
     </row>
-    <row r="215">
+    <row r="215" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K215" s="2"/>
     </row>
-    <row r="216">
+    <row r="216" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K216" s="2"/>
     </row>
-    <row r="217">
+    <row r="217" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K217" s="2"/>
     </row>
-    <row r="218">
+    <row r="218" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K218" s="2"/>
     </row>
-    <row r="219">
+    <row r="219" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K219" s="2"/>
     </row>
-    <row r="220">
+    <row r="220" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K220" s="2"/>
     </row>
-    <row r="221">
+    <row r="221" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K221" s="2"/>
     </row>
-    <row r="222">
+    <row r="222" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K222" s="2"/>
     </row>
-    <row r="223">
+    <row r="223" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K223" s="2"/>
     </row>
-    <row r="224">
+    <row r="224" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K224" s="2"/>
     </row>
-    <row r="225">
+    <row r="225" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K225" s="2"/>
     </row>
-    <row r="226">
+    <row r="226" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K226" s="2"/>
     </row>
-    <row r="227">
+    <row r="227" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K227" s="2"/>
     </row>
-    <row r="228">
+    <row r="228" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K228" s="2"/>
     </row>
-    <row r="229">
+    <row r="229" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K229" s="2"/>
     </row>
-    <row r="230">
+    <row r="230" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K230" s="2"/>
     </row>
-    <row r="231">
+    <row r="231" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K231" s="2"/>
     </row>
-    <row r="232">
+    <row r="232" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K232" s="2"/>
     </row>
-    <row r="233">
+    <row r="233" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K233" s="2"/>
     </row>
-    <row r="234">
+    <row r="234" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K234" s="2"/>
     </row>
-    <row r="235">
+    <row r="235" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K235" s="2"/>
     </row>
-    <row r="236">
+    <row r="236" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K236" s="2"/>
     </row>
-    <row r="237">
+    <row r="237" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K237" s="2"/>
     </row>
-    <row r="238">
+    <row r="238" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K238" s="2"/>
     </row>
-    <row r="239">
+    <row r="239" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K239" s="2"/>
     </row>
-    <row r="240">
+    <row r="240" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K240" s="2"/>
     </row>
-    <row r="241">
+    <row r="241" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K241" s="2"/>
     </row>
-    <row r="242">
+    <row r="242" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K242" s="2"/>
     </row>
-    <row r="243">
+    <row r="243" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K243" s="2"/>
     </row>
-    <row r="244">
+    <row r="244" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K244" s="2"/>
     </row>
-    <row r="245">
+    <row r="245" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K245" s="2"/>
     </row>
-    <row r="246">
+    <row r="246" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K246" s="2"/>
     </row>
-    <row r="247">
+    <row r="247" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K247" s="2"/>
     </row>
-    <row r="248">
+    <row r="248" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K248" s="2"/>
     </row>
-    <row r="249">
+    <row r="249" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K249" s="2"/>
     </row>
-    <row r="250">
+    <row r="250" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K250" s="2"/>
     </row>
-    <row r="251">
+    <row r="251" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K251" s="2"/>
     </row>
-    <row r="252">
+    <row r="252" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K252" s="2"/>
     </row>
-    <row r="253">
+    <row r="253" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K253" s="2"/>
     </row>
-    <row r="254">
+    <row r="254" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K254" s="2"/>
     </row>
-    <row r="255">
+    <row r="255" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K255" s="2"/>
     </row>
-    <row r="256">
+    <row r="256" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K256" s="2"/>
     </row>
-    <row r="257">
+    <row r="257" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K257" s="2"/>
     </row>
-    <row r="258">
+    <row r="258" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K258" s="2"/>
     </row>
-    <row r="259">
+    <row r="259" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K259" s="2"/>
     </row>
-    <row r="260">
+    <row r="260" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K260" s="2"/>
     </row>
-    <row r="261">
+    <row r="261" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K261" s="2"/>
     </row>
-    <row r="262">
+    <row r="262" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K262" s="2"/>
     </row>
-    <row r="263">
+    <row r="263" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K263" s="2"/>
     </row>
-    <row r="264">
+    <row r="264" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K264" s="2"/>
     </row>
-    <row r="265">
+    <row r="265" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K265" s="2"/>
     </row>
-    <row r="266">
+    <row r="266" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K266" s="2"/>
     </row>
-    <row r="267">
+    <row r="267" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K267" s="2"/>
     </row>
-    <row r="268">
+    <row r="268" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K268" s="2"/>
     </row>
-    <row r="269">
+    <row r="269" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K269" s="2"/>
     </row>
-    <row r="270">
+    <row r="270" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K270" s="2"/>
     </row>
-    <row r="271">
+    <row r="271" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K271" s="2"/>
     </row>
-    <row r="272">
+    <row r="272" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K272" s="2"/>
     </row>
-    <row r="273">
+    <row r="273" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K273" s="2"/>
     </row>
-    <row r="274">
+    <row r="274" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K274" s="2"/>
     </row>
-    <row r="275">
+    <row r="275" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K275" s="2"/>
     </row>
-    <row r="276">
+    <row r="276" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K276" s="2"/>
     </row>
-    <row r="277">
+    <row r="277" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K277" s="2"/>
     </row>
-    <row r="278">
+    <row r="278" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K278" s="2"/>
     </row>
-    <row r="279">
+    <row r="279" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K279" s="2"/>
     </row>
-    <row r="280">
+    <row r="280" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K280" s="2"/>
     </row>
-    <row r="281">
+    <row r="281" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K281" s="2"/>
     </row>
-    <row r="282">
+    <row r="282" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K282" s="2"/>
     </row>
-    <row r="283">
+    <row r="283" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K283" s="2"/>
     </row>
-    <row r="284">
+    <row r="284" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K284" s="2"/>
     </row>
-    <row r="285">
+    <row r="285" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K285" s="2"/>
     </row>
-    <row r="286">
+    <row r="286" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K286" s="2"/>
     </row>
-    <row r="287">
+    <row r="287" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K287" s="2"/>
     </row>
-    <row r="288">
+    <row r="288" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K288" s="2"/>
     </row>
-    <row r="289">
+    <row r="289" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K289" s="2"/>
     </row>
-    <row r="290">
+    <row r="290" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K290" s="2"/>
     </row>
-    <row r="291">
+    <row r="291" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K291" s="2"/>
     </row>
-    <row r="292">
+    <row r="292" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K292" s="2"/>
     </row>
-    <row r="293">
+    <row r="293" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K293" s="2"/>
     </row>
-    <row r="294">
+    <row r="294" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K294" s="2"/>
     </row>
-    <row r="295">
+    <row r="295" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K295" s="2"/>
     </row>
-    <row r="296">
+    <row r="296" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K296" s="2"/>
     </row>
-    <row r="297">
+    <row r="297" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K297" s="2"/>
     </row>
-    <row r="298">
+    <row r="298" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K298" s="2"/>
     </row>
-    <row r="299">
+    <row r="299" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K299" s="2"/>
     </row>
-    <row r="300">
+    <row r="300" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K300" s="2"/>
     </row>
-    <row r="301">
+    <row r="301" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K301" s="2"/>
     </row>
-    <row r="302">
+    <row r="302" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K302" s="2"/>
     </row>
-    <row r="303">
+    <row r="303" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K303" s="2"/>
     </row>
-    <row r="304">
+    <row r="304" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K304" s="2"/>
     </row>
-    <row r="305">
+    <row r="305" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K305" s="2"/>
     </row>
-    <row r="306">
+    <row r="306" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K306" s="2"/>
     </row>
-    <row r="307">
+    <row r="307" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K307" s="2"/>
     </row>
-    <row r="308">
+    <row r="308" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K308" s="2"/>
     </row>
-    <row r="309">
+    <row r="309" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K309" s="2"/>
     </row>
-    <row r="310">
+    <row r="310" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K310" s="2"/>
     </row>
-    <row r="311">
+    <row r="311" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K311" s="2"/>
     </row>
-    <row r="312">
+    <row r="312" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K312" s="2"/>
     </row>
-    <row r="313">
+    <row r="313" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K313" s="2"/>
     </row>
-    <row r="314">
+    <row r="314" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K314" s="2"/>
     </row>
-    <row r="315">
+    <row r="315" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K315" s="2"/>
     </row>
-    <row r="316">
+    <row r="316" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K316" s="2"/>
     </row>
-    <row r="317">
+    <row r="317" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K317" s="2"/>
     </row>
-    <row r="318">
+    <row r="318" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K318" s="2"/>
     </row>
-    <row r="319">
+    <row r="319" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K319" s="2"/>
     </row>
-    <row r="320">
+    <row r="320" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K320" s="2"/>
     </row>
-    <row r="321">
+    <row r="321" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K321" s="2"/>
     </row>
-    <row r="322">
+    <row r="322" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K322" s="2"/>
     </row>
-    <row r="323">
+    <row r="323" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K323" s="2"/>
     </row>
-    <row r="324">
+    <row r="324" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K324" s="2"/>
     </row>
-    <row r="325">
+    <row r="325" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K325" s="2"/>
     </row>
-    <row r="326">
+    <row r="326" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K326" s="2"/>
     </row>
-    <row r="327">
+    <row r="327" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K327" s="2"/>
     </row>
-    <row r="328">
+    <row r="328" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K328" s="2"/>
     </row>
-    <row r="329">
+    <row r="329" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K329" s="2"/>
     </row>
-    <row r="330">
+    <row r="330" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K330" s="2"/>
     </row>
-    <row r="331">
+    <row r="331" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K331" s="2"/>
     </row>
-    <row r="332">
+    <row r="332" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K332" s="2"/>
     </row>
-    <row r="333">
+    <row r="333" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K333" s="2"/>
     </row>
-    <row r="334">
+    <row r="334" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K334" s="2"/>
     </row>
-    <row r="335">
+    <row r="335" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K335" s="2"/>
     </row>
-    <row r="336">
+    <row r="336" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K336" s="2"/>
     </row>
-    <row r="337">
+    <row r="337" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K337" s="2"/>
     </row>
-    <row r="338">
+    <row r="338" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K338" s="2"/>
     </row>
-    <row r="339">
+    <row r="339" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K339" s="2"/>
     </row>
-    <row r="340">
+    <row r="340" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K340" s="2"/>
     </row>
-    <row r="341">
+    <row r="341" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K341" s="2"/>
     </row>
-    <row r="342">
+    <row r="342" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K342" s="2"/>
     </row>
-    <row r="343">
+    <row r="343" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K343" s="2"/>
     </row>
-    <row r="344">
+    <row r="344" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K344" s="2"/>
     </row>
-    <row r="345">
+    <row r="345" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K345" s="2"/>
     </row>
-    <row r="346">
+    <row r="346" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K346" s="2"/>
     </row>
-    <row r="347">
+    <row r="347" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K347" s="2"/>
     </row>
-    <row r="348">
+    <row r="348" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K348" s="2"/>
     </row>
-    <row r="349">
+    <row r="349" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K349" s="2"/>
     </row>
-    <row r="350">
+    <row r="350" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K350" s="2"/>
     </row>
-    <row r="351">
+    <row r="351" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K351" s="2"/>
     </row>
-    <row r="352">
+    <row r="352" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K352" s="2"/>
     </row>
-    <row r="353">
+    <row r="353" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K353" s="2"/>
     </row>
-    <row r="354">
+    <row r="354" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K354" s="2"/>
     </row>
-    <row r="355">
+    <row r="355" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K355" s="2"/>
     </row>
-    <row r="356">
+    <row r="356" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K356" s="2"/>
     </row>
-    <row r="357">
+    <row r="357" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K357" s="2"/>
     </row>
-    <row r="358">
+    <row r="358" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K358" s="2"/>
     </row>
-    <row r="359">
+    <row r="359" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K359" s="2"/>
     </row>
-    <row r="360">
+    <row r="360" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K360" s="2"/>
     </row>
-    <row r="361">
+    <row r="361" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K361" s="2"/>
     </row>
-    <row r="362">
+    <row r="362" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K362" s="2"/>
     </row>
-    <row r="363">
+    <row r="363" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K363" s="2"/>
     </row>
-    <row r="364">
+    <row r="364" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K364" s="2"/>
     </row>
-    <row r="365">
+    <row r="365" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K365" s="2"/>
     </row>
-    <row r="366">
+    <row r="366" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K366" s="2"/>
     </row>
-    <row r="367">
+    <row r="367" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K367" s="2"/>
     </row>
-    <row r="368">
+    <row r="368" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K368" s="2"/>
     </row>
-    <row r="369">
+    <row r="369" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K369" s="2"/>
     </row>
-    <row r="370">
+    <row r="370" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K370" s="2"/>
     </row>
-    <row r="371">
+    <row r="371" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K371" s="2"/>
     </row>
-    <row r="372">
+    <row r="372" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K372" s="2"/>
     </row>
-    <row r="373">
+    <row r="373" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K373" s="2"/>
     </row>
-    <row r="374">
+    <row r="374" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K374" s="2"/>
     </row>
-    <row r="375">
+    <row r="375" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K375" s="2"/>
     </row>
-    <row r="376">
+    <row r="376" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K376" s="2"/>
     </row>
-    <row r="377">
+    <row r="377" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K377" s="2"/>
     </row>
-    <row r="378">
+    <row r="378" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K378" s="2"/>
     </row>
-    <row r="379">
+    <row r="379" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K379" s="2"/>
     </row>
-    <row r="380">
+    <row r="380" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K380" s="2"/>
     </row>
-    <row r="381">
+    <row r="381" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K381" s="2"/>
     </row>
-    <row r="382">
+    <row r="382" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K382" s="2"/>
     </row>
-    <row r="383">
+    <row r="383" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K383" s="2"/>
     </row>
-    <row r="384">
+    <row r="384" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K384" s="2"/>
     </row>
-    <row r="385">
+    <row r="385" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K385" s="2"/>
     </row>
-    <row r="386">
+    <row r="386" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K386" s="2"/>
     </row>
-    <row r="387">
+    <row r="387" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K387" s="2"/>
     </row>
-    <row r="388">
+    <row r="388" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K388" s="2"/>
     </row>
-    <row r="389">
+    <row r="389" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K389" s="2"/>
     </row>
-    <row r="390">
+    <row r="390" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K390" s="2"/>
     </row>
-    <row r="391">
+    <row r="391" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K391" s="2"/>
     </row>
-    <row r="392">
+    <row r="392" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K392" s="2"/>
     </row>
-    <row r="393">
+    <row r="393" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K393" s="2"/>
     </row>
-    <row r="394">
+    <row r="394" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K394" s="2"/>
     </row>
-    <row r="395">
+    <row r="395" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K395" s="2"/>
     </row>
-    <row r="396">
+    <row r="396" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K396" s="2"/>
     </row>
-    <row r="397">
+    <row r="397" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K397" s="2"/>
     </row>
-    <row r="398">
+    <row r="398" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K398" s="2"/>
     </row>
-    <row r="399">
+    <row r="399" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K399" s="2"/>
     </row>
-    <row r="400">
+    <row r="400" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K400" s="2"/>
     </row>
-    <row r="401">
+    <row r="401" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K401" s="2"/>
     </row>
-    <row r="402">
+    <row r="402" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K402" s="2"/>
     </row>
-    <row r="403">
+    <row r="403" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K403" s="2"/>
     </row>
-    <row r="404">
+    <row r="404" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K404" s="2"/>
     </row>
-    <row r="405">
+    <row r="405" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K405" s="2"/>
     </row>
-    <row r="406">
+    <row r="406" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K406" s="2"/>
     </row>
-    <row r="407">
+    <row r="407" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K407" s="2"/>
     </row>
-    <row r="408">
+    <row r="408" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K408" s="2"/>
     </row>
-    <row r="409">
+    <row r="409" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K409" s="2"/>
     </row>
-    <row r="410">
+    <row r="410" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K410" s="2"/>
     </row>
-    <row r="411">
+    <row r="411" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K411" s="2"/>
     </row>
-    <row r="412">
+    <row r="412" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K412" s="2"/>
     </row>
-    <row r="413">
+    <row r="413" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K413" s="2"/>
     </row>
-    <row r="414">
+    <row r="414" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K414" s="2"/>
     </row>
-    <row r="415">
+    <row r="415" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K415" s="2"/>
     </row>
-    <row r="416">
+    <row r="416" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K416" s="2"/>
     </row>
-    <row r="417">
+    <row r="417" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K417" s="2"/>
     </row>
-    <row r="418">
+    <row r="418" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K418" s="2"/>
     </row>
-    <row r="419">
+    <row r="419" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K419" s="2"/>
     </row>
-    <row r="420">
+    <row r="420" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K420" s="2"/>
     </row>
-    <row r="421">
+    <row r="421" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K421" s="2"/>
     </row>
-    <row r="422">
+    <row r="422" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K422" s="2"/>
     </row>
-    <row r="423">
+    <row r="423" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K423" s="2"/>
     </row>
-    <row r="424">
+    <row r="424" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K424" s="2"/>
     </row>
-    <row r="425">
+    <row r="425" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K425" s="2"/>
     </row>
-    <row r="426">
+    <row r="426" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K426" s="2"/>
     </row>
-    <row r="427">
+    <row r="427" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K427" s="2"/>
     </row>
-    <row r="428">
+    <row r="428" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K428" s="2"/>
     </row>
-    <row r="429">
+    <row r="429" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K429" s="2"/>
     </row>
-    <row r="430">
+    <row r="430" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K430" s="2"/>
     </row>
-    <row r="431">
+    <row r="431" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K431" s="2"/>
     </row>
-    <row r="432">
+    <row r="432" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K432" s="2"/>
     </row>
-    <row r="433">
+    <row r="433" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K433" s="2"/>
     </row>
-    <row r="434">
+    <row r="434" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K434" s="2"/>
     </row>
-    <row r="435">
+    <row r="435" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K435" s="2"/>
     </row>
-    <row r="436">
+    <row r="436" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K436" s="2"/>
     </row>
-    <row r="437">
+    <row r="437" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K437" s="2"/>
     </row>
-    <row r="438">
+    <row r="438" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K438" s="2"/>
     </row>
-    <row r="439">
+    <row r="439" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K439" s="2"/>
     </row>
-    <row r="440">
+    <row r="440" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K440" s="2"/>
     </row>
-    <row r="441">
+    <row r="441" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K441" s="2"/>
     </row>
-    <row r="442">
+    <row r="442" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K442" s="2"/>
     </row>
-    <row r="443">
+    <row r="443" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K443" s="2"/>
     </row>
-    <row r="444">
+    <row r="444" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K444" s="2"/>
     </row>
-    <row r="445">
+    <row r="445" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K445" s="2"/>
     </row>
-    <row r="446">
+    <row r="446" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K446" s="2"/>
     </row>
-    <row r="447">
+    <row r="447" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K447" s="2"/>
     </row>
-    <row r="448">
+    <row r="448" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K448" s="2"/>
     </row>
-    <row r="449">
+    <row r="449" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K449" s="2"/>
     </row>
-    <row r="450">
+    <row r="450" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K450" s="2"/>
     </row>
-    <row r="451">
+    <row r="451" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K451" s="2"/>
     </row>
-    <row r="452">
+    <row r="452" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K452" s="2"/>
     </row>
-    <row r="453">
+    <row r="453" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K453" s="2"/>
     </row>
-    <row r="454">
+    <row r="454" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K454" s="2"/>
     </row>
-    <row r="455">
+    <row r="455" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K455" s="2"/>
     </row>
-    <row r="456">
+    <row r="456" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K456" s="2"/>
     </row>
-    <row r="457">
+    <row r="457" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K457" s="2"/>
     </row>
-    <row r="458">
+    <row r="458" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K458" s="2"/>
     </row>
-    <row r="459">
+    <row r="459" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K459" s="2"/>
     </row>
-    <row r="460">
+    <row r="460" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K460" s="2"/>
     </row>
-    <row r="461">
+    <row r="461" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K461" s="2"/>
     </row>
-    <row r="462">
+    <row r="462" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K462" s="2"/>
     </row>
-    <row r="463">
+    <row r="463" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K463" s="2"/>
     </row>
-    <row r="464">
+    <row r="464" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K464" s="2"/>
     </row>
-    <row r="465">
+    <row r="465" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K465" s="2"/>
     </row>
-    <row r="466">
+    <row r="466" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K466" s="2"/>
     </row>
-    <row r="467">
+    <row r="467" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K467" s="2"/>
     </row>
-    <row r="468">
+    <row r="468" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K468" s="2"/>
     </row>
-    <row r="469">
+    <row r="469" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K469" s="2"/>
     </row>
-    <row r="470">
+    <row r="470" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K470" s="2"/>
     </row>
-    <row r="471">
+    <row r="471" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K471" s="2"/>
     </row>
-    <row r="472">
+    <row r="472" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K472" s="2"/>
     </row>
-    <row r="473">
+    <row r="473" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K473" s="2"/>
     </row>
-    <row r="474">
+    <row r="474" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K474" s="2"/>
     </row>
-    <row r="475">
+    <row r="475" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K475" s="2"/>
     </row>
-    <row r="476">
+    <row r="476" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K476" s="2"/>
     </row>
-    <row r="477">
+    <row r="477" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K477" s="2"/>
     </row>
-    <row r="478">
+    <row r="478" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K478" s="2"/>
     </row>
-    <row r="479">
+    <row r="479" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K479" s="2"/>
     </row>
-    <row r="480">
+    <row r="480" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K480" s="2"/>
     </row>
-    <row r="481">
+    <row r="481" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K481" s="2"/>
     </row>
-    <row r="482">
+    <row r="482" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K482" s="2"/>
     </row>
-    <row r="483">
+    <row r="483" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K483" s="2"/>
     </row>
-    <row r="484">
+    <row r="484" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K484" s="2"/>
     </row>
-    <row r="485">
+    <row r="485" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K485" s="2"/>
     </row>
-    <row r="486">
+    <row r="486" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K486" s="2"/>
     </row>
-    <row r="487">
+    <row r="487" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K487" s="2"/>
     </row>
-    <row r="488">
+    <row r="488" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K488" s="2"/>
     </row>
-    <row r="489">
+    <row r="489" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K489" s="2"/>
     </row>
-    <row r="490">
+    <row r="490" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K490" s="2"/>
     </row>
-    <row r="491">
+    <row r="491" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K491" s="2"/>
     </row>
-    <row r="492">
+    <row r="492" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K492" s="2"/>
     </row>
-    <row r="493">
+    <row r="493" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K493" s="2"/>
     </row>
-    <row r="494">
+    <row r="494" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K494" s="2"/>
     </row>
-    <row r="495">
+    <row r="495" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K495" s="2"/>
     </row>
-    <row r="496">
+    <row r="496" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K496" s="2"/>
     </row>
-    <row r="497">
+    <row r="497" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K497" s="2"/>
     </row>
-    <row r="498">
+    <row r="498" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K498" s="2"/>
     </row>
-    <row r="499">
+    <row r="499" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K499" s="2"/>
     </row>
-    <row r="500">
+    <row r="500" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K500" s="2"/>
     </row>
-    <row r="501">
+    <row r="501" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K501" s="2"/>
     </row>
-    <row r="502">
+    <row r="502" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K502" s="2"/>
     </row>
-    <row r="503">
+    <row r="503" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K503" s="2"/>
     </row>
-    <row r="504">
+    <row r="504" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K504" s="2"/>
     </row>
-    <row r="505">
+    <row r="505" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K505" s="2"/>
     </row>
-    <row r="506">
+    <row r="506" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K506" s="2"/>
     </row>
-    <row r="507">
+    <row r="507" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K507" s="2"/>
     </row>
-    <row r="508">
+    <row r="508" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K508" s="2"/>
     </row>
-    <row r="509">
+    <row r="509" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K509" s="2"/>
     </row>
-    <row r="510">
+    <row r="510" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K510" s="2"/>
     </row>
-    <row r="511">
+    <row r="511" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K511" s="2"/>
     </row>
-    <row r="512">
+    <row r="512" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K512" s="2"/>
     </row>
-    <row r="513">
+    <row r="513" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K513" s="2"/>
     </row>
-    <row r="514">
+    <row r="514" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K514" s="2"/>
     </row>
-    <row r="515">
+    <row r="515" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K515" s="2"/>
     </row>
-    <row r="516">
+    <row r="516" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K516" s="2"/>
     </row>
-    <row r="517">
+    <row r="517" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K517" s="2"/>
     </row>
-    <row r="518">
+    <row r="518" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K518" s="2"/>
     </row>
-    <row r="519">
+    <row r="519" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K519" s="2"/>
     </row>
-    <row r="520">
+    <row r="520" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K520" s="2"/>
     </row>
-    <row r="521">
+    <row r="521" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K521" s="2"/>
     </row>
-    <row r="522">
+    <row r="522" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K522" s="2"/>
     </row>
-    <row r="523">
+    <row r="523" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K523" s="2"/>
     </row>
-    <row r="524">
+    <row r="524" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K524" s="2"/>
     </row>
-    <row r="525">
+    <row r="525" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K525" s="2"/>
     </row>
-    <row r="526">
+    <row r="526" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K526" s="2"/>
     </row>
-    <row r="527">
+    <row r="527" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K527" s="2"/>
     </row>
-    <row r="528">
+    <row r="528" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K528" s="2"/>
     </row>
-    <row r="529">
+    <row r="529" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K529" s="2"/>
     </row>
-    <row r="530">
+    <row r="530" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K530" s="2"/>
     </row>
-    <row r="531">
+    <row r="531" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K531" s="2"/>
     </row>
-    <row r="532">
+    <row r="532" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K532" s="2"/>
     </row>
-    <row r="533">
+    <row r="533" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K533" s="2"/>
     </row>
-    <row r="534">
+    <row r="534" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K534" s="2"/>
     </row>
-    <row r="535">
+    <row r="535" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K535" s="2"/>
     </row>
-    <row r="536">
+    <row r="536" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K536" s="2"/>
     </row>
-    <row r="537">
+    <row r="537" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K537" s="2"/>
     </row>
-    <row r="538">
+    <row r="538" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K538" s="2"/>
     </row>
-    <row r="539">
+    <row r="539" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K539" s="2"/>
     </row>
-    <row r="540">
+    <row r="540" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K540" s="2"/>
     </row>
-    <row r="541">
+    <row r="541" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K541" s="2"/>
     </row>
-    <row r="542">
+    <row r="542" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K542" s="2"/>
     </row>
-    <row r="543">
+    <row r="543" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K543" s="2"/>
     </row>
-    <row r="544">
+    <row r="544" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K544" s="2"/>
     </row>
-    <row r="545">
+    <row r="545" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K545" s="2"/>
     </row>
-    <row r="546">
+    <row r="546" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K546" s="2"/>
     </row>
-    <row r="547">
+    <row r="547" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K547" s="2"/>
     </row>
-    <row r="548">
+    <row r="548" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K548" s="2"/>
     </row>
-    <row r="549">
+    <row r="549" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K549" s="2"/>
     </row>
-    <row r="550">
+    <row r="550" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K550" s="2"/>
     </row>
-    <row r="551">
+    <row r="551" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K551" s="2"/>
     </row>
-    <row r="552">
+    <row r="552" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K552" s="2"/>
     </row>
-    <row r="553">
+    <row r="553" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K553" s="2"/>
     </row>
-    <row r="554">
+    <row r="554" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K554" s="2"/>
     </row>
-    <row r="555">
+    <row r="555" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K555" s="2"/>
     </row>
-    <row r="556">
+    <row r="556" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K556" s="2"/>
     </row>
-    <row r="557">
+    <row r="557" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K557" s="2"/>
     </row>
-    <row r="558">
+    <row r="558" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K558" s="2"/>
     </row>
-    <row r="559">
+    <row r="559" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K559" s="2"/>
     </row>
-    <row r="560">
+    <row r="560" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K560" s="2"/>
     </row>
-    <row r="561">
+    <row r="561" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K561" s="2"/>
     </row>
-    <row r="562">
+    <row r="562" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K562" s="2"/>
     </row>
-    <row r="563">
+    <row r="563" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K563" s="2"/>
     </row>
-    <row r="564">
+    <row r="564" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K564" s="2"/>
     </row>
-    <row r="565">
+    <row r="565" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K565" s="2"/>
     </row>
-    <row r="566">
+    <row r="566" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K566" s="2"/>
     </row>
-    <row r="567">
+    <row r="567" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K567" s="2"/>
     </row>
-    <row r="568">
+    <row r="568" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K568" s="2"/>
     </row>
-    <row r="569">
+    <row r="569" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K569" s="2"/>
     </row>
-    <row r="570">
+    <row r="570" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K570" s="2"/>
     </row>
-    <row r="571">
+    <row r="571" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K571" s="2"/>
     </row>
-    <row r="572">
+    <row r="572" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K572" s="2"/>
     </row>
-    <row r="573">
+    <row r="573" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K573" s="2"/>
     </row>
-    <row r="574">
+    <row r="574" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K574" s="2"/>
     </row>
-    <row r="575">
+    <row r="575" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K575" s="2"/>
     </row>
-    <row r="576">
+    <row r="576" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K576" s="2"/>
     </row>
-    <row r="577">
+    <row r="577" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K577" s="2"/>
     </row>
-    <row r="578">
+    <row r="578" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K578" s="2"/>
     </row>
-    <row r="579">
+    <row r="579" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K579" s="2"/>
     </row>
-    <row r="580">
+    <row r="580" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K580" s="2"/>
     </row>
-    <row r="581">
+    <row r="581" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K581" s="2"/>
     </row>
-    <row r="582">
+    <row r="582" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K582" s="2"/>
     </row>
-    <row r="583">
+    <row r="583" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K583" s="2"/>
     </row>
-    <row r="584">
+    <row r="584" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K584" s="2"/>
     </row>
-    <row r="585">
+    <row r="585" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K585" s="2"/>
     </row>
-    <row r="586">
+    <row r="586" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K586" s="2"/>
     </row>
-    <row r="587">
+    <row r="587" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K587" s="2"/>
     </row>
-    <row r="588">
+    <row r="588" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K588" s="2"/>
     </row>
-    <row r="589">
+    <row r="589" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K589" s="2"/>
     </row>
-    <row r="590">
+    <row r="590" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K590" s="2"/>
     </row>
-    <row r="591">
+    <row r="591" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K591" s="2"/>
     </row>
-    <row r="592">
+    <row r="592" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K592" s="2"/>
     </row>
-    <row r="593">
+    <row r="593" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K593" s="2"/>
     </row>
-    <row r="594">
+    <row r="594" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K594" s="2"/>
     </row>
-    <row r="595">
+    <row r="595" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K595" s="2"/>
     </row>
-    <row r="596">
+    <row r="596" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K596" s="2"/>
     </row>
-    <row r="597">
+    <row r="597" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K597" s="2"/>
     </row>
-    <row r="598">
+    <row r="598" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K598" s="2"/>
     </row>
-    <row r="599">
+    <row r="599" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K599" s="2"/>
     </row>
-    <row r="600">
+    <row r="600" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K600" s="2"/>
     </row>
-    <row r="601">
+    <row r="601" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K601" s="2"/>
     </row>
-    <row r="602">
+    <row r="602" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K602" s="2"/>
     </row>
-    <row r="603">
+    <row r="603" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K603" s="2"/>
     </row>
-    <row r="604">
+    <row r="604" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K604" s="2"/>
     </row>
-    <row r="605">
+    <row r="605" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K605" s="2"/>
     </row>
-    <row r="606">
+    <row r="606" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K606" s="2"/>
     </row>
-    <row r="607">
+    <row r="607" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K607" s="2"/>
     </row>
-    <row r="608">
+    <row r="608" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K608" s="2"/>
     </row>
-    <row r="609">
+    <row r="609" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K609" s="2"/>
     </row>
-    <row r="610">
+    <row r="610" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K610" s="2"/>
     </row>
-    <row r="611">
+    <row r="611" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K611" s="2"/>
     </row>
-    <row r="612">
+    <row r="612" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K612" s="2"/>
     </row>
-    <row r="613">
+    <row r="613" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K613" s="2"/>
     </row>
-    <row r="614">
+    <row r="614" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K614" s="2"/>
     </row>
-    <row r="615">
+    <row r="615" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K615" s="2"/>
     </row>
-    <row r="616">
+    <row r="616" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K616" s="2"/>
     </row>
-    <row r="617">
+    <row r="617" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K617" s="2"/>
     </row>
-    <row r="618">
+    <row r="618" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K618" s="2"/>
     </row>
-    <row r="619">
+    <row r="619" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K619" s="2"/>
     </row>
-    <row r="620">
+    <row r="620" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K620" s="2"/>
     </row>
-    <row r="621">
+    <row r="621" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K621" s="2"/>
     </row>
-    <row r="622">
+    <row r="622" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K622" s="2"/>
     </row>
-    <row r="623">
+    <row r="623" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K623" s="2"/>
     </row>
-    <row r="624">
+    <row r="624" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K624" s="2"/>
     </row>
-    <row r="625">
+    <row r="625" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K625" s="2"/>
     </row>
-    <row r="626">
+    <row r="626" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K626" s="2"/>
     </row>
-    <row r="627">
+    <row r="627" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K627" s="2"/>
     </row>
-    <row r="628">
+    <row r="628" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K628" s="2"/>
     </row>
-    <row r="629">
+    <row r="629" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K629" s="2"/>
     </row>
-    <row r="630">
+    <row r="630" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K630" s="2"/>
     </row>
-    <row r="631">
+    <row r="631" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K631" s="2"/>
     </row>
-    <row r="632">
+    <row r="632" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K632" s="2"/>
     </row>
-    <row r="633">
+    <row r="633" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K633" s="2"/>
     </row>
-    <row r="634">
+    <row r="634" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K634" s="2"/>
     </row>
-    <row r="635">
+    <row r="635" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K635" s="2"/>
     </row>
-    <row r="636">
+    <row r="636" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K636" s="2"/>
     </row>
-    <row r="637">
+    <row r="637" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K637" s="2"/>
     </row>
-    <row r="638">
+    <row r="638" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K638" s="2"/>
     </row>
-    <row r="639">
+    <row r="639" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K639" s="2"/>
     </row>
-    <row r="640">
+    <row r="640" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K640" s="2"/>
     </row>
-    <row r="641">
+    <row r="641" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K641" s="2"/>
     </row>
-    <row r="642">
+    <row r="642" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K642" s="2"/>
     </row>
-    <row r="643">
+    <row r="643" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K643" s="2"/>
     </row>
-    <row r="644">
+    <row r="644" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K644" s="2"/>
     </row>
-    <row r="645">
+    <row r="645" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K645" s="2"/>
     </row>
-    <row r="646">
+    <row r="646" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K646" s="2"/>
     </row>
-    <row r="647">
+    <row r="647" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K647" s="2"/>
     </row>
-    <row r="648">
+    <row r="648" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K648" s="2"/>
     </row>
-    <row r="649">
+    <row r="649" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K649" s="2"/>
     </row>
-    <row r="650">
+    <row r="650" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K650" s="2"/>
     </row>
-    <row r="651">
+    <row r="651" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K651" s="2"/>
     </row>
-    <row r="652">
+    <row r="652" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K652" s="2"/>
     </row>
-    <row r="653">
+    <row r="653" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K653" s="2"/>
     </row>
-    <row r="654">
+    <row r="654" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K654" s="2"/>
     </row>
-    <row r="655">
+    <row r="655" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K655" s="2"/>
     </row>
-    <row r="656">
+    <row r="656" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K656" s="2"/>
     </row>
-    <row r="657">
+    <row r="657" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K657" s="2"/>
     </row>
-    <row r="658">
+    <row r="658" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K658" s="2"/>
     </row>
-    <row r="659">
+    <row r="659" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K659" s="2"/>
     </row>
-    <row r="660">
+    <row r="660" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K660" s="2"/>
     </row>
-    <row r="661">
+    <row r="661" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K661" s="2"/>
     </row>
-    <row r="662">
+    <row r="662" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K662" s="2"/>
     </row>
-    <row r="663">
+    <row r="663" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K663" s="2"/>
     </row>
-    <row r="664">
+    <row r="664" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K664" s="2"/>
     </row>
-    <row r="665">
+    <row r="665" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K665" s="2"/>
     </row>
-    <row r="666">
+    <row r="666" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K666" s="2"/>
     </row>
-    <row r="667">
+    <row r="667" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K667" s="2"/>
     </row>
-    <row r="668">
+    <row r="668" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K668" s="2"/>
     </row>
-    <row r="669">
+    <row r="669" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K669" s="2"/>
     </row>
-    <row r="670">
+    <row r="670" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K670" s="2"/>
     </row>
-    <row r="671">
+    <row r="671" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K671" s="2"/>
     </row>
-    <row r="672">
+    <row r="672" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K672" s="2"/>
     </row>
-    <row r="673">
+    <row r="673" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K673" s="2"/>
     </row>
-    <row r="674">
+    <row r="674" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K674" s="2"/>
     </row>
-    <row r="675">
+    <row r="675" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K675" s="2"/>
     </row>
-    <row r="676">
+    <row r="676" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K676" s="2"/>
     </row>
-    <row r="677">
+    <row r="677" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K677" s="2"/>
     </row>
-    <row r="678">
+    <row r="678" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K678" s="2"/>
     </row>
-    <row r="679">
+    <row r="679" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K679" s="2"/>
     </row>
-    <row r="680">
+    <row r="680" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K680" s="2"/>
     </row>
-    <row r="681">
+    <row r="681" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K681" s="2"/>
     </row>
-    <row r="682">
+    <row r="682" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K682" s="2"/>
     </row>
-    <row r="683">
+    <row r="683" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K683" s="2"/>
     </row>
-    <row r="684">
+    <row r="684" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K684" s="2"/>
     </row>
-    <row r="685">
+    <row r="685" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K685" s="2"/>
     </row>
-    <row r="686">
+    <row r="686" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K686" s="2"/>
     </row>
-    <row r="687">
+    <row r="687" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K687" s="2"/>
     </row>
-    <row r="688">
+    <row r="688" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K688" s="2"/>
     </row>
-    <row r="689">
+    <row r="689" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K689" s="2"/>
     </row>
-    <row r="690">
+    <row r="690" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K690" s="2"/>
     </row>
-    <row r="691">
+    <row r="691" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K691" s="2"/>
     </row>
-    <row r="692">
+    <row r="692" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K692" s="2"/>
     </row>
-    <row r="693">
+    <row r="693" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K693" s="2"/>
     </row>
-    <row r="694">
+    <row r="694" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K694" s="2"/>
     </row>
-    <row r="695">
+    <row r="695" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K695" s="2"/>
     </row>
-    <row r="696">
+    <row r="696" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K696" s="2"/>
     </row>
-    <row r="697">
+    <row r="697" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K697" s="2"/>
     </row>
-    <row r="698">
+    <row r="698" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K698" s="2"/>
     </row>
-    <row r="699">
+    <row r="699" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K699" s="2"/>
     </row>
-    <row r="700">
+    <row r="700" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K700" s="2"/>
     </row>
-    <row r="701">
+    <row r="701" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K701" s="2"/>
     </row>
-    <row r="702">
+    <row r="702" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K702" s="2"/>
     </row>
-    <row r="703">
+    <row r="703" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K703" s="2"/>
     </row>
-    <row r="704">
+    <row r="704" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K704" s="2"/>
     </row>
-    <row r="705">
+    <row r="705" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K705" s="2"/>
     </row>
-    <row r="706">
+    <row r="706" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K706" s="2"/>
     </row>
-    <row r="707">
+    <row r="707" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K707" s="2"/>
     </row>
-    <row r="708">
+    <row r="708" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K708" s="2"/>
     </row>
-    <row r="709">
+    <row r="709" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K709" s="2"/>
     </row>
-    <row r="710">
+    <row r="710" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K710" s="2"/>
     </row>
-    <row r="711">
+    <row r="711" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K711" s="2"/>
     </row>
-    <row r="712">
+    <row r="712" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K712" s="2"/>
     </row>
-    <row r="713">
+    <row r="713" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K713" s="2"/>
     </row>
-    <row r="714">
+    <row r="714" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K714" s="2"/>
     </row>
-    <row r="715">
+    <row r="715" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K715" s="2"/>
     </row>
-    <row r="716">
+    <row r="716" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K716" s="2"/>
     </row>
-    <row r="717">
+    <row r="717" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K717" s="2"/>
     </row>
-    <row r="718">
+    <row r="718" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K718" s="2"/>
     </row>
-    <row r="719">
+    <row r="719" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K719" s="2"/>
     </row>
-    <row r="720">
+    <row r="720" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K720" s="2"/>
     </row>
-    <row r="721">
+    <row r="721" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K721" s="2"/>
     </row>
-    <row r="722">
+    <row r="722" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K722" s="2"/>
     </row>
-    <row r="723">
+    <row r="723" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K723" s="2"/>
     </row>
-    <row r="724">
+    <row r="724" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K724" s="2"/>
     </row>
-    <row r="725">
+    <row r="725" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K725" s="2"/>
     </row>
-    <row r="726">
+    <row r="726" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K726" s="2"/>
     </row>
-    <row r="727">
+    <row r="727" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K727" s="2"/>
     </row>
-    <row r="728">
+    <row r="728" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K728" s="2"/>
     </row>
-    <row r="729">
+    <row r="729" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K729" s="2"/>
     </row>
-    <row r="730">
+    <row r="730" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K730" s="2"/>
     </row>
-    <row r="731">
+    <row r="731" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K731" s="2"/>
     </row>
-    <row r="732">
+    <row r="732" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K732" s="2"/>
     </row>
-    <row r="733">
+    <row r="733" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K733" s="2"/>
     </row>
-    <row r="734">
+    <row r="734" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K734" s="2"/>
     </row>
-    <row r="735">
+    <row r="735" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K735" s="2"/>
     </row>
-    <row r="736">
+    <row r="736" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K736" s="2"/>
     </row>
-    <row r="737">
+    <row r="737" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K737" s="2"/>
     </row>
-    <row r="738">
+    <row r="738" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K738" s="2"/>
     </row>
-    <row r="739">
+    <row r="739" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K739" s="2"/>
     </row>
-    <row r="740">
+    <row r="740" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K740" s="2"/>
     </row>
-    <row r="741">
+    <row r="741" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K741" s="2"/>
     </row>
-    <row r="742">
+    <row r="742" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K742" s="2"/>
     </row>
-    <row r="743">
+    <row r="743" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K743" s="2"/>
     </row>
-    <row r="744">
+    <row r="744" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K744" s="2"/>
     </row>
-    <row r="745">
+    <row r="745" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K745" s="2"/>
     </row>
-    <row r="746">
+    <row r="746" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K746" s="2"/>
     </row>
-    <row r="747">
+    <row r="747" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K747" s="2"/>
     </row>
-    <row r="748">
+    <row r="748" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K748" s="2"/>
     </row>
-    <row r="749">
+    <row r="749" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K749" s="2"/>
     </row>
-    <row r="750">
+    <row r="750" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K750" s="2"/>
     </row>
-    <row r="751">
+    <row r="751" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K751" s="2"/>
     </row>
-    <row r="752">
+    <row r="752" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K752" s="2"/>
     </row>
-    <row r="753">
+    <row r="753" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K753" s="2"/>
     </row>
-    <row r="754">
+    <row r="754" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K754" s="2"/>
     </row>
-    <row r="755">
+    <row r="755" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K755" s="2"/>
     </row>
-    <row r="756">
+    <row r="756" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K756" s="2"/>
     </row>
-    <row r="757">
+    <row r="757" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K757" s="2"/>
     </row>
-    <row r="758">
+    <row r="758" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K758" s="2"/>
     </row>
-    <row r="759">
+    <row r="759" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K759" s="2"/>
     </row>
-    <row r="760">
+    <row r="760" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K760" s="2"/>
     </row>
-    <row r="761">
+    <row r="761" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K761" s="2"/>
     </row>
-    <row r="762">
+    <row r="762" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K762" s="2"/>
     </row>
-    <row r="763">
+    <row r="763" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K763" s="2"/>
     </row>
-    <row r="764">
+    <row r="764" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K764" s="2"/>
     </row>
-    <row r="765">
+    <row r="765" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K765" s="2"/>
     </row>
-    <row r="766">
+    <row r="766" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K766" s="2"/>
     </row>
-    <row r="767">
+    <row r="767" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K767" s="2"/>
     </row>
-    <row r="768">
+    <row r="768" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K768" s="2"/>
     </row>
-    <row r="769">
+    <row r="769" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K769" s="2"/>
     </row>
-    <row r="770">
+    <row r="770" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K770" s="2"/>
     </row>
-    <row r="771">
+    <row r="771" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K771" s="2"/>
     </row>
-    <row r="772">
+    <row r="772" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K772" s="2"/>
     </row>
-    <row r="773">
+    <row r="773" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K773" s="2"/>
     </row>
-    <row r="774">
+    <row r="774" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K774" s="2"/>
     </row>
-    <row r="775">
+    <row r="775" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K775" s="2"/>
     </row>
-    <row r="776">
+    <row r="776" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K776" s="2"/>
     </row>
-    <row r="777">
+    <row r="777" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K777" s="2"/>
     </row>
-    <row r="778">
+    <row r="778" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K778" s="2"/>
     </row>
-    <row r="779">
+    <row r="779" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K779" s="2"/>
     </row>
-    <row r="780">
+    <row r="780" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K780" s="2"/>
     </row>
-    <row r="781">
+    <row r="781" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K781" s="2"/>
     </row>
-    <row r="782">
+    <row r="782" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K782" s="2"/>
     </row>
-    <row r="783">
+    <row r="783" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K783" s="2"/>
     </row>
-    <row r="784">
+    <row r="784" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K784" s="2"/>
     </row>
-    <row r="785">
+    <row r="785" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K785" s="2"/>
     </row>
-    <row r="786">
+    <row r="786" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K786" s="2"/>
     </row>
-    <row r="787">
+    <row r="787" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K787" s="2"/>
     </row>
-    <row r="788">
+    <row r="788" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K788" s="2"/>
     </row>
-    <row r="789">
+    <row r="789" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K789" s="2"/>
     </row>
-    <row r="790">
+    <row r="790" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K790" s="2"/>
     </row>
-    <row r="791">
+    <row r="791" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K791" s="2"/>
     </row>
-    <row r="792">
+    <row r="792" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K792" s="2"/>
     </row>
-    <row r="793">
+    <row r="793" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K793" s="2"/>
     </row>
-    <row r="794">
+    <row r="794" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K794" s="2"/>
     </row>
-    <row r="795">
+    <row r="795" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K795" s="2"/>
     </row>
-    <row r="796">
+    <row r="796" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K796" s="2"/>
     </row>
-    <row r="797">
+    <row r="797" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K797" s="2"/>
     </row>
-    <row r="798">
+    <row r="798" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K798" s="2"/>
     </row>
-    <row r="799">
+    <row r="799" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K799" s="2"/>
     </row>
-    <row r="800">
+    <row r="800" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K800" s="2"/>
     </row>
-    <row r="801">
+    <row r="801" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K801" s="2"/>
     </row>
-    <row r="802">
+    <row r="802" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K802" s="2"/>
     </row>
-    <row r="803">
+    <row r="803" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K803" s="2"/>
     </row>
-    <row r="804">
+    <row r="804" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K804" s="2"/>
     </row>
-    <row r="805">
+    <row r="805" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K805" s="2"/>
     </row>
-    <row r="806">
+    <row r="806" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K806" s="2"/>
     </row>
-    <row r="807">
+    <row r="807" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K807" s="2"/>
     </row>
-    <row r="808">
+    <row r="808" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K808" s="2"/>
     </row>
-    <row r="809">
+    <row r="809" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K809" s="2"/>
     </row>
-    <row r="810">
+    <row r="810" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K810" s="2"/>
     </row>
-    <row r="811">
+    <row r="811" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K811" s="2"/>
     </row>
-    <row r="812">
+    <row r="812" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K812" s="2"/>
     </row>
-    <row r="813">
+    <row r="813" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K813" s="2"/>
     </row>
-    <row r="814">
+    <row r="814" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K814" s="2"/>
     </row>
-    <row r="815">
+    <row r="815" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K815" s="2"/>
     </row>
-    <row r="816">
+    <row r="816" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K816" s="2"/>
     </row>
-    <row r="817">
+    <row r="817" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K817" s="2"/>
     </row>
-    <row r="818">
+    <row r="818" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K818" s="2"/>
     </row>
-    <row r="819">
+    <row r="819" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K819" s="2"/>
     </row>
-    <row r="820">
+    <row r="820" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K820" s="2"/>
     </row>
-    <row r="821">
+    <row r="821" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K821" s="2"/>
     </row>
-    <row r="822">
+    <row r="822" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K822" s="2"/>
     </row>
-    <row r="823">
+    <row r="823" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K823" s="2"/>
     </row>
-    <row r="824">
+    <row r="824" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K824" s="2"/>
     </row>
-    <row r="825">
+    <row r="825" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K825" s="2"/>
     </row>
-    <row r="826">
+    <row r="826" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K826" s="2"/>
     </row>
-    <row r="827">
+    <row r="827" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K827" s="2"/>
     </row>
-    <row r="828">
+    <row r="828" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K828" s="2"/>
     </row>
-    <row r="829">
+    <row r="829" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K829" s="2"/>
     </row>
-    <row r="830">
+    <row r="830" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K830" s="2"/>
     </row>
-    <row r="831">
+    <row r="831" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K831" s="2"/>
     </row>
-    <row r="832">
+    <row r="832" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K832" s="2"/>
     </row>
-    <row r="833">
+    <row r="833" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K833" s="2"/>
     </row>
-    <row r="834">
+    <row r="834" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K834" s="2"/>
     </row>
-    <row r="835">
+    <row r="835" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K835" s="2"/>
     </row>
-    <row r="836">
+    <row r="836" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K836" s="2"/>
     </row>
-    <row r="837">
+    <row r="837" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K837" s="2"/>
     </row>
-    <row r="838">
+    <row r="838" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K838" s="2"/>
     </row>
-    <row r="839">
+    <row r="839" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K839" s="2"/>
     </row>
-    <row r="840">
+    <row r="840" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K840" s="2"/>
     </row>
-    <row r="841">
+    <row r="841" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K841" s="2"/>
     </row>
-    <row r="842">
+    <row r="842" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K842" s="2"/>
     </row>
-    <row r="843">
+    <row r="843" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K843" s="2"/>
     </row>
-    <row r="844">
+    <row r="844" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K844" s="2"/>
     </row>
-    <row r="845">
+    <row r="845" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K845" s="2"/>
     </row>
-    <row r="846">
+    <row r="846" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K846" s="2"/>
     </row>
-    <row r="847">
+    <row r="847" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K847" s="2"/>
     </row>
-    <row r="848">
+    <row r="848" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K848" s="2"/>
     </row>
-    <row r="849">
+    <row r="849" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K849" s="2"/>
     </row>
-    <row r="850">
+    <row r="850" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K850" s="2"/>
     </row>
-    <row r="851">
+    <row r="851" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K851" s="2"/>
     </row>
-    <row r="852">
+    <row r="852" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K852" s="2"/>
     </row>
-    <row r="853">
+    <row r="853" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K853" s="2"/>
     </row>
-    <row r="854">
+    <row r="854" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K854" s="2"/>
     </row>
-    <row r="855">
+    <row r="855" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K855" s="2"/>
     </row>
-    <row r="856">
+    <row r="856" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K856" s="2"/>
     </row>
-    <row r="857">
+    <row r="857" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K857" s="2"/>
     </row>
-    <row r="858">
+    <row r="858" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K858" s="2"/>
     </row>
-    <row r="859">
+    <row r="859" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K859" s="2"/>
     </row>
-    <row r="860">
+    <row r="860" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K860" s="2"/>
     </row>
-    <row r="861">
+    <row r="861" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K861" s="2"/>
     </row>
-    <row r="862">
+    <row r="862" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K862" s="2"/>
     </row>
-    <row r="863">
+    <row r="863" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K863" s="2"/>
     </row>
-    <row r="864">
+    <row r="864" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K864" s="2"/>
     </row>
-    <row r="865">
+    <row r="865" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K865" s="2"/>
     </row>
-    <row r="866">
+    <row r="866" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K866" s="2"/>
     </row>
-    <row r="867">
+    <row r="867" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K867" s="2"/>
     </row>
-    <row r="868">
+    <row r="868" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K868" s="2"/>
     </row>
-    <row r="869">
+    <row r="869" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K869" s="2"/>
     </row>
-    <row r="870">
+    <row r="870" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K870" s="2"/>
     </row>
-    <row r="871">
+    <row r="871" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K871" s="2"/>
     </row>
-    <row r="872">
+    <row r="872" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K872" s="2"/>
     </row>
-    <row r="873">
+    <row r="873" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K873" s="2"/>
     </row>
-    <row r="874">
+    <row r="874" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K874" s="2"/>
     </row>
-    <row r="875">
+    <row r="875" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K875" s="2"/>
     </row>
-    <row r="876">
+    <row r="876" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K876" s="2"/>
     </row>
-    <row r="877">
+    <row r="877" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K877" s="2"/>
     </row>
-    <row r="878">
+    <row r="878" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K878" s="2"/>
     </row>
-    <row r="879">
+    <row r="879" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K879" s="2"/>
     </row>
-    <row r="880">
+    <row r="880" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K880" s="2"/>
     </row>
-    <row r="881">
+    <row r="881" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K881" s="2"/>
     </row>
-    <row r="882">
+    <row r="882" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K882" s="2"/>
     </row>
-    <row r="883">
+    <row r="883" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K883" s="2"/>
     </row>
-    <row r="884">
+    <row r="884" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K884" s="2"/>
     </row>
-    <row r="885">
+    <row r="885" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K885" s="2"/>
     </row>
-    <row r="886">
+    <row r="886" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K886" s="2"/>
     </row>
-    <row r="887">
+    <row r="887" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K887" s="2"/>
     </row>
-    <row r="888">
+    <row r="888" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K888" s="2"/>
     </row>
-    <row r="889">
+    <row r="889" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K889" s="2"/>
     </row>
-    <row r="890">
+    <row r="890" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K890" s="2"/>
     </row>
-    <row r="891">
+    <row r="891" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K891" s="2"/>
     </row>
-    <row r="892">
+    <row r="892" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K892" s="2"/>
     </row>
-    <row r="893">
+    <row r="893" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K893" s="2"/>
     </row>
-    <row r="894">
+    <row r="894" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K894" s="2"/>
     </row>
-    <row r="895">
+    <row r="895" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K895" s="2"/>
     </row>
-    <row r="896">
+    <row r="896" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K896" s="2"/>
     </row>
-    <row r="897">
+    <row r="897" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K897" s="2"/>
     </row>
-    <row r="898">
+    <row r="898" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K898" s="2"/>
     </row>
-    <row r="899">
+    <row r="899" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K899" s="2"/>
     </row>
-    <row r="900">
+    <row r="900" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K900" s="2"/>
     </row>
-    <row r="901">
+    <row r="901" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K901" s="2"/>
     </row>
-    <row r="902">
+    <row r="902" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K902" s="2"/>
     </row>
-    <row r="903">
+    <row r="903" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K903" s="2"/>
     </row>
-    <row r="904">
+    <row r="904" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K904" s="2"/>
     </row>
-    <row r="905">
+    <row r="905" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K905" s="2"/>
     </row>
-    <row r="906">
+    <row r="906" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K906" s="2"/>
     </row>
-    <row r="907">
+    <row r="907" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K907" s="2"/>
     </row>
-    <row r="908">
+    <row r="908" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K908" s="2"/>
     </row>
-    <row r="909">
+    <row r="909" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K909" s="2"/>
     </row>
-    <row r="910">
+    <row r="910" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K910" s="2"/>
     </row>
-    <row r="911">
+    <row r="911" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K911" s="2"/>
     </row>
-    <row r="912">
+    <row r="912" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K912" s="2"/>
     </row>
-    <row r="913">
+    <row r="913" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K913" s="2"/>
     </row>
-    <row r="914">
+    <row r="914" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K914" s="2"/>
     </row>
-    <row r="915">
+    <row r="915" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K915" s="2"/>
     </row>
-    <row r="916">
+    <row r="916" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K916" s="2"/>
     </row>
-    <row r="917">
+    <row r="917" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K917" s="2"/>
     </row>
-    <row r="918">
+    <row r="918" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K918" s="2"/>
     </row>
-    <row r="919">
+    <row r="919" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K919" s="2"/>
     </row>
-    <row r="920">
+    <row r="920" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K920" s="2"/>
     </row>
-    <row r="921">
+    <row r="921" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K921" s="2"/>
     </row>
-    <row r="922">
+    <row r="922" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K922" s="2"/>
     </row>
-    <row r="923">
+    <row r="923" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K923" s="2"/>
     </row>
-    <row r="924">
+    <row r="924" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K924" s="2"/>
     </row>
-    <row r="925">
+    <row r="925" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K925" s="2"/>
     </row>
-    <row r="926">
+    <row r="926" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K926" s="2"/>
     </row>
-    <row r="927">
+    <row r="927" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K927" s="2"/>
     </row>
-    <row r="928">
+    <row r="928" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K928" s="2"/>
     </row>
-    <row r="929">
+    <row r="929" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K929" s="2"/>
     </row>
-    <row r="930">
+    <row r="930" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K930" s="2"/>
     </row>
-    <row r="931">
+    <row r="931" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K931" s="2"/>
     </row>
-    <row r="932">
+    <row r="932" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K932" s="2"/>
     </row>
-    <row r="933">
+    <row r="933" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K933" s="2"/>
     </row>
-    <row r="934">
+    <row r="934" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K934" s="2"/>
     </row>
-    <row r="935">
+    <row r="935" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K935" s="2"/>
     </row>
-    <row r="936">
+    <row r="936" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K936" s="2"/>
     </row>
-    <row r="937">
+    <row r="937" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K937" s="2"/>
     </row>
-    <row r="938">
+    <row r="938" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K938" s="2"/>
     </row>
-    <row r="939">
+    <row r="939" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K939" s="2"/>
     </row>
-    <row r="940">
+    <row r="940" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K940" s="2"/>
     </row>
-    <row r="941">
+    <row r="941" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K941" s="2"/>
     </row>
-    <row r="942">
+    <row r="942" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K942" s="2"/>
     </row>
-    <row r="943">
+    <row r="943" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K943" s="2"/>
     </row>
-    <row r="944">
+    <row r="944" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K944" s="2"/>
     </row>
-    <row r="945">
+    <row r="945" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K945" s="2"/>
     </row>
-    <row r="946">
+    <row r="946" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K946" s="2"/>
     </row>
-    <row r="947">
+    <row r="947" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K947" s="2"/>
     </row>
-    <row r="948">
+    <row r="948" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K948" s="2"/>
     </row>
-    <row r="949">
+    <row r="949" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K949" s="2"/>
     </row>
-    <row r="950">
+    <row r="950" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K950" s="2"/>
     </row>
-    <row r="951">
+    <row r="951" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K951" s="2"/>
     </row>
-    <row r="952">
+    <row r="952" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K952" s="2"/>
     </row>
-    <row r="953">
+    <row r="953" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K953" s="2"/>
     </row>
-    <row r="954">
+    <row r="954" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K954" s="2"/>
     </row>
-    <row r="955">
+    <row r="955" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K955" s="2"/>
     </row>
-    <row r="956">
+    <row r="956" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K956" s="2"/>
     </row>
-    <row r="957">
+    <row r="957" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K957" s="2"/>
     </row>
-    <row r="958">
+    <row r="958" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K958" s="2"/>
     </row>
-    <row r="959">
+    <row r="959" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K959" s="2"/>
     </row>
-    <row r="960">
+    <row r="960" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K960" s="2"/>
     </row>
-    <row r="961">
+    <row r="961" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K961" s="2"/>
     </row>
-    <row r="962">
+    <row r="962" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K962" s="2"/>
     </row>
-    <row r="963">
+    <row r="963" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K963" s="2"/>
     </row>
-    <row r="964">
+    <row r="964" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K964" s="2"/>
     </row>
-    <row r="965">
+    <row r="965" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K965" s="2"/>
     </row>
-    <row r="966">
+    <row r="966" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K966" s="2"/>
     </row>
-    <row r="967">
+    <row r="967" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K967" s="2"/>
     </row>
-    <row r="968">
+    <row r="968" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K968" s="2"/>
     </row>
-    <row r="969">
+    <row r="969" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K969" s="2"/>
     </row>
-    <row r="970">
+    <row r="970" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K970" s="2"/>
     </row>
-    <row r="971">
+    <row r="971" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K971" s="2"/>
     </row>
-    <row r="972">
+    <row r="972" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K972" s="2"/>
     </row>
-    <row r="973">
+    <row r="973" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K973" s="2"/>
     </row>
-    <row r="974">
+    <row r="974" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K974" s="2"/>
     </row>
-    <row r="975">
+    <row r="975" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K975" s="2"/>
     </row>
-    <row r="976">
+    <row r="976" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K976" s="2"/>
     </row>
-    <row r="977">
+    <row r="977" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K977" s="2"/>
     </row>
-    <row r="978">
+    <row r="978" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K978" s="2"/>
     </row>
-    <row r="979">
+    <row r="979" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K979" s="2"/>
     </row>
-    <row r="980">
+    <row r="980" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K980" s="2"/>
     </row>
-    <row r="981">
+    <row r="981" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K981" s="2"/>
     </row>
-    <row r="982">
+    <row r="982" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K982" s="2"/>
     </row>
-    <row r="983">
+    <row r="983" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K983" s="2"/>
     </row>
-    <row r="984">
+    <row r="984" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K984" s="2"/>
     </row>
-    <row r="985">
+    <row r="985" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K985" s="2"/>
     </row>
-    <row r="986">
+    <row r="986" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K986" s="2"/>
     </row>
-    <row r="987">
+    <row r="987" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K987" s="2"/>
     </row>
-    <row r="988">
+    <row r="988" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K988" s="2"/>
     </row>
-    <row r="989">
+    <row r="989" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K989" s="2"/>
     </row>
-    <row r="990">
+    <row r="990" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K990" s="2"/>
     </row>
-    <row r="991">
+    <row r="991" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K991" s="2"/>
     </row>
-    <row r="992">
+    <row r="992" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K992" s="2"/>
     </row>
-    <row r="993">
+    <row r="993" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K993" s="2"/>
     </row>
-    <row r="994">
+    <row r="994" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K994" s="2"/>
     </row>
-    <row r="995">
+    <row r="995" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K995" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>